<commit_message>
changement de la description 6d330fc57501e2dd85417689fbb5a24e90d2d745
</commit_message>
<xml_diff>
--- a/FL-gt-structure/ig/CodeSystem-fr-core-cs-type-activite.xlsx
+++ b/FL-gt-structure/ig/CodeSystem-fr-core-cs-type-activite.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-11-02T22:07:39+00:00</t>
+    <t>2025-12-02T20:15:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -87,7 +87,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>La nomenclature des types d'activité.</t>
+    <t>La nomenclature des types d'activité de la terminologie SAE (Statistique Annuelle des Etablissements de santé) maintenue par la DREES.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>